<commit_message>
update readme + images
</commit_message>
<xml_diff>
--- a/Tugas9/test.xlsx
+++ b/Tugas9/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maranatha\Documents\Kuliah\SEM 6\Progjar\Progjar_B\Tugas9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2098DBCF-0A5C-40C1-BFC3-4088E3583F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB46DD0-B71F-4081-9BDE-999A1918C359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6945" yWindow="1995" windowWidth="21600" windowHeight="11835" xr2:uid="{32D69AAA-BF30-484A-BC28-531B95FE3D6A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t xml:space="preserve">Concurrency level </t>
   </si>
@@ -61,12 +61,18 @@
   <si>
     <t xml:space="preserve">Transfer rate (Kbytes/sec) </t>
   </si>
+  <si>
+    <t>Async</t>
+  </si>
+  <si>
+    <t>Thread</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +83,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -116,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -124,7 +136,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B990F95-621F-4259-8A62-B7A03FABBA60}">
-  <dimension ref="B2:J10"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +478,22 @@
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -487,7 +522,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -495,28 +531,29 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>1120.538</v>
       </c>
       <c r="E3" s="1">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>1360</v>
+        <v>122000</v>
       </c>
       <c r="H3" s="1">
-        <v>221.87</v>
+        <v>0.89</v>
       </c>
       <c r="I3" s="1">
-        <v>4.5069999999999997</v>
+        <v>1120.538</v>
       </c>
       <c r="J3" s="1">
-        <v>29.47</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -524,28 +561,29 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>513.75599999999997</v>
       </c>
       <c r="E4" s="1">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>1360</v>
+        <v>122000</v>
       </c>
       <c r="H4" s="1">
-        <v>263.76</v>
+        <v>1.95</v>
       </c>
       <c r="I4" s="1">
-        <v>3.7909999999999999</v>
+        <v>513.75599999999997</v>
       </c>
       <c r="J4" s="1">
-        <v>35.03</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -553,43 +591,59 @@
         <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>424.589</v>
       </c>
       <c r="E5" s="1">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>1360</v>
+        <v>122000</v>
       </c>
       <c r="H5" s="1">
-        <v>276.51</v>
+        <v>2.36</v>
       </c>
       <c r="I5" s="1">
-        <v>36.164999999999999</v>
+        <v>424.589</v>
       </c>
       <c r="J5" s="1">
-        <v>36.72</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>20</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>518.48199999999997</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>122000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.93</v>
+      </c>
+      <c r="I6" s="1">
+        <v>518.48199999999997</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -597,28 +651,29 @@
         <v>30</v>
       </c>
       <c r="D7" s="1">
-        <v>0.29699999999999999</v>
+        <v>451.59399999999999</v>
       </c>
       <c r="E7" s="1">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>6800</v>
+        <v>122000</v>
       </c>
       <c r="H7" s="1">
-        <v>168.5</v>
+        <v>2.21</v>
       </c>
       <c r="I7" s="1">
-        <v>178.04400000000001</v>
+        <v>451.59399999999999</v>
       </c>
       <c r="J7" s="1">
-        <v>22.38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -626,28 +681,29 @@
         <v>50</v>
       </c>
       <c r="D8" s="1">
-        <v>0.28499999999999998</v>
+        <v>541.99099999999999</v>
       </c>
       <c r="E8" s="1">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>6800</v>
+        <v>122000</v>
       </c>
       <c r="H8" s="1">
-        <v>175.23</v>
+        <v>1.85</v>
       </c>
       <c r="I8" s="1">
-        <v>285.34699999999998</v>
+        <v>541.99099999999999</v>
       </c>
       <c r="J8" s="1">
-        <v>23.27</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -655,41 +711,352 @@
         <v>100</v>
       </c>
       <c r="D9" s="1">
-        <v>0.90600000000000003</v>
+        <v>442.51100000000002</v>
       </c>
       <c r="E9" s="1">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>13600</v>
+        <v>122000</v>
       </c>
       <c r="H9" s="1">
-        <v>110.33</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="I9" s="1">
-        <v>906.38199999999995</v>
+        <v>442.51100000000002</v>
       </c>
       <c r="J9" s="1">
-        <v>14.65</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="2">
         <v>200</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="D10" s="4">
+        <v>1.575</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="4">
+        <v>143</v>
+      </c>
+      <c r="G10" s="4">
+        <v>17446</v>
+      </c>
+      <c r="H10" s="4">
+        <v>635.05999999999995</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1.575</v>
+      </c>
+      <c r="J10" s="4">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.5670000000000002</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>122000</v>
+      </c>
+      <c r="H14" s="1">
+        <v>280.31</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3.5670000000000002</v>
+      </c>
+      <c r="J14" s="1">
+        <v>33.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.835</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>122000</v>
+      </c>
+      <c r="H15" s="1">
+        <v>352.69</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2.835</v>
+      </c>
+      <c r="J15" s="1">
+        <v>42.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.649</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>122000</v>
+      </c>
+      <c r="H16" s="1">
+        <v>377.5</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2.649</v>
+      </c>
+      <c r="J16" s="1">
+        <v>44.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.5070000000000001</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>122000</v>
+      </c>
+      <c r="H17" s="1">
+        <v>398.92</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2.5070000000000001</v>
+      </c>
+      <c r="J17" s="1">
+        <v>47.53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.8180000000000001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>122000</v>
+      </c>
+      <c r="H18" s="1">
+        <v>540.04</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1.8180000000000001</v>
+      </c>
+      <c r="J18" s="1">
+        <v>65.53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.845</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>122000</v>
+      </c>
+      <c r="H19" s="1">
+        <v>541.89</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1.845</v>
+      </c>
+      <c r="J19" s="1">
+        <v>64.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <v>100</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.8160000000000001</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>122000</v>
+      </c>
+      <c r="H20" s="1">
+        <v>550.64</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1.8160000000000001</v>
+      </c>
+      <c r="J20" s="1">
+        <v>65.599999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2">
+        <v>200</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F21" s="1">
+        <v>157</v>
+      </c>
+      <c r="G21" s="1">
+        <v>19154</v>
+      </c>
+      <c r="H21" s="4">
+        <v>3374.79</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="J21" s="4">
+        <v>63.13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>